<commit_message>
updated new login page and navbar
</commit_message>
<xml_diff>
--- a/WW_Customer_DATA.xlsx
+++ b/WW_Customer_DATA.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\W27969\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/navneeth/Desktop/WEB/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B11A5602-0ECA-4CD7-899F-2B83EBD74E32}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5CE56BA-2448-4348-9AA9-C126AD6D1A4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="NeededByXML" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,20 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">NeededByXML!$A$1:$B$83</definedName>
   </definedNames>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -523,7 +536,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -660,7 +673,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -843,6 +856,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1022,11 +1041,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1381,20 +1401,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="B44" sqref="B44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.33203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="53.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1402,7 +1422,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -1410,7 +1430,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
@@ -1418,7 +1438,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>7</v>
       </c>
@@ -1426,7 +1446,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -1434,7 +1454,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="2" t="s">
         <v>11</v>
       </c>
@@ -1442,7 +1462,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -1450,7 +1470,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -1458,7 +1478,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
         <v>17</v>
       </c>
@@ -1466,7 +1486,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
         <v>18</v>
       </c>
@@ -1474,7 +1494,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
         <v>20</v>
       </c>
@@ -1482,7 +1502,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
         <v>23</v>
       </c>
@@ -1490,7 +1510,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
         <v>25</v>
       </c>
@@ -1498,7 +1518,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
         <v>27</v>
       </c>
@@ -1506,7 +1526,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
         <v>29</v>
       </c>
@@ -1514,7 +1534,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>31</v>
       </c>
@@ -1522,7 +1542,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
         <v>33</v>
       </c>
@@ -1530,7 +1550,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
         <v>35</v>
       </c>
@@ -1538,7 +1558,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>37</v>
       </c>
@@ -1546,7 +1566,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1554,7 +1574,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>41</v>
       </c>
@@ -1562,7 +1582,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>43</v>
       </c>
@@ -1570,7 +1590,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
         <v>45</v>
       </c>
@@ -1578,7 +1598,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
         <v>47</v>
       </c>
@@ -1586,7 +1606,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
         <v>49</v>
       </c>
@@ -1594,7 +1614,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
         <v>51</v>
       </c>
@@ -1602,7 +1622,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
         <v>53</v>
       </c>
@@ -1610,7 +1630,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
         <v>55</v>
       </c>
@@ -1618,7 +1638,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
         <v>57</v>
       </c>
@@ -1626,7 +1646,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
         <v>59</v>
       </c>
@@ -1634,7 +1654,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
         <v>61</v>
       </c>
@@ -1642,7 +1662,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
         <v>63</v>
       </c>
@@ -1650,7 +1670,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
         <v>65</v>
       </c>
@@ -1658,7 +1678,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="2" t="s">
         <v>67</v>
       </c>
@@ -1666,7 +1686,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="2" t="s">
         <v>69</v>
       </c>
@@ -1674,7 +1694,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="2" t="s">
         <v>71</v>
       </c>
@@ -1682,7 +1702,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="2" t="s">
         <v>73</v>
       </c>
@@ -1690,7 +1710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="2" t="s">
         <v>75</v>
       </c>
@@ -1698,7 +1718,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="2" t="s">
         <v>77</v>
       </c>
@@ -1706,7 +1726,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="2" t="s">
         <v>79</v>
       </c>
@@ -1714,7 +1734,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>81</v>
       </c>
@@ -1722,7 +1742,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="2" t="s">
         <v>83</v>
       </c>
@@ -1730,7 +1750,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="43" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="2" t="s">
         <v>85</v>
       </c>
@@ -1738,7 +1758,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="44" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="2" t="s">
         <v>87</v>
       </c>
@@ -1746,7 +1766,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="2" t="s">
         <v>89</v>
       </c>
@@ -1754,7 +1774,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="46" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="2" t="s">
         <v>91</v>
       </c>
@@ -1762,7 +1782,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="2" t="s">
         <v>93</v>
       </c>
@@ -1770,7 +1790,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="48" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="2" t="s">
         <v>95</v>
       </c>
@@ -1778,7 +1798,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="2" t="s">
         <v>97</v>
       </c>
@@ -1786,7 +1806,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="3" t="s">
         <v>99</v>
       </c>
@@ -1794,7 +1814,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="2" t="s">
         <v>101</v>
       </c>
@@ -1802,7 +1822,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="2" t="s">
         <v>103</v>
       </c>
@@ -1810,7 +1830,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="2" t="s">
         <v>105</v>
       </c>
@@ -1818,7 +1838,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="2" t="s">
         <v>107</v>
       </c>
@@ -1826,7 +1846,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="2" t="s">
         <v>109</v>
       </c>
@@ -1834,7 +1854,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="2" t="s">
         <v>111</v>
       </c>
@@ -1842,7 +1862,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="2" t="s">
         <v>113</v>
       </c>
@@ -1850,7 +1870,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="2" t="s">
         <v>115</v>
       </c>
@@ -1858,7 +1878,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="2" t="s">
         <v>117</v>
       </c>
@@ -1866,7 +1886,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="2" t="s">
         <v>119</v>
       </c>
@@ -1874,7 +1894,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="2" t="s">
         <v>121</v>
       </c>
@@ -1882,7 +1902,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="2" t="s">
         <v>123</v>
       </c>
@@ -1890,7 +1910,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="2" t="s">
         <v>125</v>
       </c>
@@ -1898,7 +1918,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="2" t="s">
         <v>127</v>
       </c>
@@ -1906,7 +1926,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="2" t="s">
         <v>129</v>
       </c>
@@ -1914,7 +1934,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="2" t="s">
         <v>131</v>
       </c>
@@ -1922,7 +1942,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="2" t="s">
         <v>133</v>
       </c>
@@ -1930,7 +1950,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="2" t="s">
         <v>135</v>
       </c>
@@ -1938,7 +1958,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="2" t="s">
         <v>137</v>
       </c>
@@ -1946,7 +1966,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="2" t="s">
         <v>139</v>
       </c>
@@ -1954,7 +1974,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="2" t="s">
         <v>141</v>
       </c>
@@ -1962,7 +1982,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="2" t="s">
         <v>143</v>
       </c>
@@ -1970,15 +1990,15 @@
         <v>144</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A73" s="2" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A73" s="4" t="s">
         <v>145</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="4" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="2" t="s">
         <v>147</v>
       </c>
@@ -1986,15 +2006,15 @@
         <v>148</v>
       </c>
     </row>
-    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A75" s="2" t="s">
+    <row r="75" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A75" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="3" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="2" t="s">
         <v>151</v>
       </c>
@@ -2002,7 +2022,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="2" t="s">
         <v>153</v>
       </c>
@@ -2010,7 +2030,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="2" t="s">
         <v>155</v>
       </c>
@@ -2018,7 +2038,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="2" t="s">
         <v>157</v>
       </c>
@@ -2026,7 +2046,7 @@
         <v>158</v>
       </c>
     </row>
-    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="2" t="s">
         <v>159</v>
       </c>
@@ -2034,7 +2054,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="2" t="s">
         <v>161</v>
       </c>
@@ -2042,7 +2062,7 @@
         <v>162</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="2" t="s">
         <v>22</v>
       </c>
@@ -2050,7 +2070,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="2" t="s">
         <v>164</v>
       </c>
@@ -2059,7 +2079,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:B83"/>
+  <autoFilter ref="A1:B83" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>